<commit_message>
finaliza dicionário de dados para o sistema
</commit_message>
<xml_diff>
--- a/diagramaER/dicionarioDados.xlsx
+++ b/diagramaER/dicionarioDados.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ads\Challenge1\SalesPop\diagramaER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DE83D87-9D68-4051-8B09-F009A8078293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E939A2-EDA3-4088-902E-08D8558C7D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{C311E320-A5B1-46E9-97C8-8614B40C887E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TABELAS" sheetId="1" r:id="rId1"/>
+    <sheet name="ATRIBUTOS" sheetId="2" r:id="rId2"/>
+    <sheet name="RELACIONAMENTO" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="132">
   <si>
     <t>Tabela</t>
   </si>
@@ -299,6 +299,141 @@
   </si>
   <si>
     <t>Número de identificação do usuário,  gerado automaticamente</t>
+  </si>
+  <si>
+    <t>Cookie-Pagina</t>
+  </si>
+  <si>
+    <t>Nome do usuário</t>
+  </si>
+  <si>
+    <t>email do usuário</t>
+  </si>
+  <si>
+    <t>telefone do usuário</t>
+  </si>
+  <si>
+    <t>empresa na qual o usuário trabalha</t>
+  </si>
+  <si>
+    <t>cargo do usuário na empresa onde trabalha</t>
+  </si>
+  <si>
+    <t>Número de identificação do atendente,  gerado automaticamente</t>
+  </si>
+  <si>
+    <t>nome do atendente</t>
+  </si>
+  <si>
+    <t>data de nascimento do atendente</t>
+  </si>
+  <si>
+    <t>telefone do atendente</t>
+  </si>
+  <si>
+    <t>email do atendente</t>
+  </si>
+  <si>
+    <t>Número de identificação do chat, gerado automaticamente</t>
+  </si>
+  <si>
+    <t>modo de operação do chat: pode ser controlado pelo bot ou pelo atendente</t>
+  </si>
+  <si>
+    <t>Avalia se o chat está ou não disponível</t>
+  </si>
+  <si>
+    <t>Chave estrangeira</t>
+  </si>
+  <si>
+    <t>Chave estrangeira da tabela auxiliar</t>
+  </si>
+  <si>
+    <t>Número de identificação do formulário de contato, gerado automaticamente</t>
+  </si>
+  <si>
+    <t>Data do preenchimento do formulário</t>
+  </si>
+  <si>
+    <t>Número de identificação do cookie, gerado automaticamente</t>
+  </si>
+  <si>
+    <t>Nome do cookie</t>
+  </si>
+  <si>
+    <t>domínio ao qual o cookie pertence</t>
+  </si>
+  <si>
+    <t>data de expiração do cookie</t>
+  </si>
+  <si>
+    <t>Idioma do site</t>
+  </si>
+  <si>
+    <t>Chave Estrageira</t>
+  </si>
+  <si>
+    <t>Número de anúncios acessados durante a sessão</t>
+  </si>
+  <si>
+    <t>Tempo de navegação no site durante a sessão</t>
+  </si>
+  <si>
+    <t>Número de identificação do das preferências do usuário, gerado automaticamente</t>
+  </si>
+  <si>
+    <t>Tipo de dautonismo do usuário, se houver</t>
+  </si>
+  <si>
+    <t>Ativa ou não modo de alto contraste</t>
+  </si>
+  <si>
+    <t>Ativa ou não links sublinhados no site</t>
+  </si>
+  <si>
+    <t>Endereço da Página, chave primária</t>
+  </si>
+  <si>
+    <t>Título da página</t>
+  </si>
+  <si>
+    <t>Conteúdo de texto presente na página</t>
+  </si>
+  <si>
+    <t>preferências de estilo css para a página</t>
+  </si>
+  <si>
+    <t>Usuário usa o chatbot ou o chat com atendente, dependendo do modo do chat</t>
+  </si>
+  <si>
+    <t>Usuários são atendidos por atendentes</t>
+  </si>
+  <si>
+    <t>Usuário pode preencher o formulário com suas informações</t>
+  </si>
+  <si>
+    <t>Usuário pode aceitar ou não cada cookie do site</t>
+  </si>
+  <si>
+    <t>Usuário define suas preferências de acessiblidade</t>
+  </si>
+  <si>
+    <t>O usuário realiza uma pesquisa dentro de alguma página</t>
+  </si>
+  <si>
+    <t>O atendente responde o usuário dentro do chat</t>
+  </si>
+  <si>
+    <t>Atendentes atendem os usuários (atendentes específicos são designados a usuários específicos)</t>
+  </si>
+  <si>
+    <t>Especialização da tabela cookie</t>
+  </si>
+  <si>
+    <t>Os cookies podem fazer alterações nas págians dependendo de sua ativação pelo usuário</t>
+  </si>
+  <si>
+    <t>As preferências de acessibilidade podem fazer alterações na página (eg. Links sublinhados)</t>
   </si>
 </sst>
 </file>
@@ -376,35 +511,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,14 +862,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57DB89E0-6084-48CC-9430-B9E41CD18151}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C2:C29"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="27.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -746,338 +888,325 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="5"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="5"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="12" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5" t="s">
+      <c r="A26" s="11"/>
+      <c r="B26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="5"/>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="12" t="s">
+      <c r="A28" s="10"/>
+      <c r="B28" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5" t="s">
+      <c r="A29" s="11"/>
+      <c r="B29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="A30" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1096,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7064F2F0-37BD-4489-81BD-8949320A0A60}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1135,121 +1264,127 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="G2" s="12" t="s">
+      <c r="F2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" s="3"/>
+      <c r="F3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" s="3"/>
+      <c r="F4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="G5" s="3"/>
+      <c r="F5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" s="3"/>
+      <c r="F6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>73</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" s="5"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" t="s">
         <v>72</v>
       </c>
       <c r="D8" t="s">
@@ -1258,80 +1393,94 @@
       <c r="E8" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>85</v>
+      <c r="F8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
+      <c r="A9" s="10"/>
       <c r="B9" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>85</v>
+      <c r="F9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
+      <c r="A10" s="10"/>
       <c r="B10" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" t="s">
         <v>74</v>
       </c>
       <c r="D10" t="s">
         <v>81</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>85</v>
+      <c r="F10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
+      <c r="A11" s="10"/>
       <c r="B11" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>85</v>
+      <c r="F11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>73</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G12" s="5"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" t="s">
         <v>72</v>
       </c>
       <c r="D13" t="s">
@@ -1340,46 +1489,55 @@
       <c r="E13" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="12" t="s">
-        <v>85</v>
+      <c r="F13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
+      <c r="A14" s="10"/>
       <c r="B14" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>85</v>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
+      <c r="A15" s="10"/>
       <c r="B15" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="12" t="s">
-        <v>85</v>
+      <c r="F15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
+      <c r="A16" s="10"/>
       <c r="B16" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" t="s">
         <v>72</v>
       </c>
       <c r="D16" t="s">
@@ -1388,16 +1546,19 @@
       <c r="E16" t="s">
         <v>84</v>
       </c>
-      <c r="F16" s="12" t="s">
-        <v>85</v>
+      <c r="F16" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
+      <c r="A17" s="10"/>
       <c r="B17" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" t="s">
         <v>72</v>
       </c>
       <c r="D17" t="s">
@@ -1406,29 +1567,32 @@
       <c r="E17" t="s">
         <v>84</v>
       </c>
-      <c r="F17" s="12" t="s">
-        <v>85</v>
+      <c r="F17" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="5"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B19" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" t="s">
         <v>72</v>
       </c>
       <c r="D19" t="s">
@@ -1437,262 +1601,302 @@
       <c r="E19" t="s">
         <v>84</v>
       </c>
-      <c r="F19" s="12" t="s">
-        <v>85</v>
+      <c r="F19" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="11"/>
+      <c r="B20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" s="5"/>
+      <c r="F20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B21" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" t="s">
         <v>72</v>
       </c>
       <c r="D21" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" t="s">
         <v>83</v>
       </c>
-      <c r="F21" s="12" t="s">
-        <v>85</v>
+      <c r="F21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
+      <c r="A22" s="10"/>
       <c r="B22" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" t="s">
         <v>74</v>
       </c>
       <c r="D22" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="12" t="s">
-        <v>85</v>
+      <c r="F22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="11"/>
+      <c r="B23" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G23" s="5"/>
+      <c r="F23" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B24" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" t="s">
         <v>72</v>
       </c>
       <c r="D24" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" t="s">
         <v>83</v>
       </c>
-      <c r="F24" s="12" t="s">
-        <v>85</v>
+      <c r="F24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
+      <c r="A25" s="10"/>
       <c r="B25" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" t="s">
         <v>79</v>
       </c>
-      <c r="F25" s="12" t="s">
-        <v>85</v>
+      <c r="F25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
+      <c r="A26" s="10"/>
       <c r="B26" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" t="s">
         <v>79</v>
       </c>
-      <c r="F26" s="12" t="s">
-        <v>85</v>
+      <c r="F26" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
+      <c r="A27" s="10"/>
       <c r="B27" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" t="s">
         <v>79</v>
       </c>
-      <c r="F27" s="12" t="s">
-        <v>85</v>
+      <c r="F27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5" t="s">
+      <c r="A28" s="11"/>
+      <c r="B28" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G28" s="5"/>
+      <c r="F28" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B29" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" t="s">
         <v>73</v>
       </c>
       <c r="D29" t="s">
         <v>77</v>
       </c>
-      <c r="F29" s="12" t="s">
-        <v>85</v>
+      <c r="F29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5" t="s">
+      <c r="A30" s="11"/>
+      <c r="B30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G30" s="5"/>
+      <c r="F30" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B31" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="12" t="s">
-        <v>85</v>
+      <c r="F31" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="11"/>
+      <c r="B32" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G32" s="5"/>
+      <c r="F32" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B33" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="3" t="s">
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" t="s">
         <v>79</v>
       </c>
-      <c r="F33" s="12" t="s">
-        <v>85</v>
+      <c r="F33" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
+      <c r="A34" s="10"/>
       <c r="B34" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" t="s">
         <v>72</v>
       </c>
       <c r="D34" t="s">
@@ -1701,18 +1905,21 @@
       <c r="E34" t="s">
         <v>84</v>
       </c>
-      <c r="F34" s="12" t="s">
-        <v>85</v>
+      <c r="F34" t="s">
+        <v>85</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B35" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" t="s">
         <v>72</v>
       </c>
       <c r="D35" t="s">
@@ -1721,121 +1928,140 @@
       <c r="E35" t="s">
         <v>84</v>
       </c>
-      <c r="F35" s="12" t="s">
-        <v>85</v>
+      <c r="F35" t="s">
+        <v>85</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="10"/>
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="7"/>
+      <c r="B36" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F36" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G36" s="5"/>
+      <c r="F36" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B37" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" t="s">
         <v>72</v>
       </c>
       <c r="D37" t="s">
         <v>77</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" t="s">
         <v>83</v>
       </c>
-      <c r="F37" s="12" t="s">
-        <v>85</v>
+      <c r="F37" t="s">
+        <v>85</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
+      <c r="A38" s="10"/>
       <c r="B38" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="12" t="s">
-        <v>75</v>
+      <c r="C38" t="s">
+        <v>73</v>
       </c>
       <c r="D38" t="s">
-        <v>78</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>85</v>
+        <v>79</v>
+      </c>
+      <c r="F38" t="s">
+        <v>85</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
+      <c r="A39" s="10"/>
       <c r="B39" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" t="s">
         <v>75</v>
       </c>
       <c r="D39" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="12" t="s">
-        <v>85</v>
+      <c r="F39" t="s">
+        <v>85</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
+      <c r="A40" s="10"/>
       <c r="B40" t="s">
         <v>68</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" t="s">
         <v>75</v>
       </c>
       <c r="D40" t="s">
         <v>78</v>
       </c>
-      <c r="F40" s="12" t="s">
-        <v>85</v>
+      <c r="F40" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
-      <c r="B41" s="5" t="s">
+      <c r="A41" s="11"/>
+      <c r="B41" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F41" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G41" s="5"/>
+      <c r="F41" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B42" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" t="s">
         <v>73</v>
       </c>
       <c r="D42" t="s">
@@ -1844,59 +2070,73 @@
       <c r="E42" t="s">
         <v>83</v>
       </c>
-      <c r="F42" s="12" t="s">
-        <v>85</v>
+      <c r="F42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="2"/>
+      <c r="A43" s="12"/>
       <c r="B43" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" t="s">
         <v>73</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="12" t="s">
-        <v>85</v>
+      <c r="F43" t="s">
+        <v>85</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="4"/>
+      <c r="A44" s="12"/>
       <c r="B44" t="s">
         <v>70</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" t="s">
         <v>79</v>
       </c>
-      <c r="F44" s="12" t="s">
-        <v>85</v>
+      <c r="F44" t="s">
+        <v>85</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="12"/>
       <c r="B45" t="s">
         <v>71</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C45" t="s">
         <v>73</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" t="s">
         <v>79</v>
       </c>
-      <c r="F45" s="12" t="s">
-        <v>85</v>
+      <c r="F45" t="s">
+        <v>85</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="12"/>
       <c r="B46" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" t="s">
         <v>72</v>
       </c>
       <c r="D46" t="s">
@@ -1905,15 +2145,19 @@
       <c r="E46" t="s">
         <v>84</v>
       </c>
-      <c r="F46" s="12" t="s">
-        <v>85</v>
+      <c r="F46" t="s">
+        <v>85</v>
+      </c>
+      <c r="G46" s="13" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="12"/>
       <c r="B47" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" t="s">
         <v>72</v>
       </c>
       <c r="D47" t="s">
@@ -1922,23 +2166,29 @@
       <c r="E47" t="s">
         <v>84</v>
       </c>
-      <c r="F47" s="12" t="s">
-        <v>85</v>
-      </c>
+      <c r="F47" t="s">
+        <v>85</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="1048576" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G1048576" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A42:A47"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A24:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1947,13 +2197,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA52D6F1-B7FB-447E-AEBD-7576C1730E15}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D1048561"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1971,146 +2226,209 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="15" t="s">
         <v>16</v>
       </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="15" t="s">
         <v>23</v>
       </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>11</v>
+      <c r="A10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>23</v>
+      <c r="A11" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>12</v>
+      <c r="A12" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>12</v>
+      <c r="A13" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="A14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="A15" s="15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>16</v>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="1048561" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1048561" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D13:D14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>